<commit_message>
Add winners and comments to test-results
</commit_message>
<xml_diff>
--- a/spec/fixtures/test-data/test-results.xlsx
+++ b/spec/fixtures/test-data/test-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="460" windowWidth="15360" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="101">
   <si>
     <t>A3</t>
   </si>
@@ -312,6 +312,21 @@
   </si>
   <si>
     <t>spotid</t>
+  </si>
+  <si>
+    <t>firstComments</t>
+  </si>
+  <si>
+    <t>secondComments</t>
+  </si>
+  <si>
+    <t>winnerID</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
   </si>
 </sst>
 </file>
@@ -333,12 +348,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -353,15 +374,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -678,7 +741,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,365 +751,600 @@
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="E25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
@@ -1056,54 +1354,90 @@
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.25">
@@ -1113,11 +1447,20 @@
       <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.25">
@@ -1127,15 +1470,24 @@
       <c r="B32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D1048576 E1:G2 F3:F32">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>